<commit_message>
Added ability to optionally lemmatise words
</commit_message>
<xml_diff>
--- a/reference/top1000_words.xlsx
+++ b/reference/top1000_words.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Code\translate_horizon_zero_dawn\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03E4542-020F-4332-8518-41C65084FBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B55B6E0-B496-418D-B690-1649CD228D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="28800" windowHeight="15345" xr2:uid="{D5063641-65F4-2742-8EC5-B146F51B679D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{D5063641-65F4-2742-8EC5-B146F51B679D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1009</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2028" uniqueCount="1145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="1146">
   <si>
     <t>rank</t>
   </si>
@@ -3469,6 +3472,9 @@
   </si>
   <si>
     <t>un'altra</t>
+  </si>
+  <si>
+    <t>grazia</t>
   </si>
 </sst>
 </file>
@@ -3819,9 +3825,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA7CEE4-5526-2447-9751-B1E3CA33BC4A}">
-  <dimension ref="A1:D1009"/>
+  <dimension ref="A1:D1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A963" workbookViewId="0">
+      <selection activeCell="D1007" sqref="D1007"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -17951,7 +17959,22 @@
         <v>1142</v>
       </c>
     </row>
+    <row r="1010" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1010">
+        <v>1009</v>
+      </c>
+      <c r="B1010" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C1010" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D1010" t="s">
+        <v>1142</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:D1009" xr:uid="{EAA7CEE4-5526-2447-9751-B1E3CA33BC4A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>